<commit_message>
mml patient information module
</commit_message>
<xml_diff>
--- a/mapping/mml_name_mapping.xlsx
+++ b/mapping/mml_name_mapping.xlsx
@@ -634,7 +634,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -642,7 +642,7 @@
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="14.125" customWidth="1"/>
     <col min="5" max="5" width="11.625" customWidth="1"/>
-    <col min="8" max="8" width="18.25" customWidth="1"/>
+    <col min="8" max="8" width="26.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.15">
@@ -751,7 +751,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="27" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>